<commit_message>
Challenge 2 and 3 ready, 1 updated
</commit_message>
<xml_diff>
--- a/00_Data/01_bike_sales/02_wrangled_data/sales_by_year.xlsx
+++ b/00_Data/01_bike_sales/02_wrangled_data/sales_by_year.xlsx
@@ -383,7 +383,7 @@
       </c>
       <c r="C2" t="inlineStr">
         <is>
-          <t>9.930.282 â‚¬</t>
+          <t>9.930.282 €</t>
         </is>
       </c>
     </row>
@@ -396,7 +396,7 @@
       </c>
       <c r="C3" t="inlineStr">
         <is>
-          <t>10.730.507 â‚¬</t>
+          <t>10.730.507 €</t>
         </is>
       </c>
     </row>
@@ -409,7 +409,7 @@
       </c>
       <c r="C4" t="inlineStr">
         <is>
-          <t>14.510.291 â‚¬</t>
+          <t>14.510.291 €</t>
         </is>
       </c>
     </row>
@@ -422,7 +422,7 @@
       </c>
       <c r="C5" t="inlineStr">
         <is>
-          <t>12.241.853 â‚¬</t>
+          <t>12.241.853 €</t>
         </is>
       </c>
     </row>
@@ -435,7 +435,7 @@
       </c>
       <c r="C6" t="inlineStr">
         <is>
-          <t>15.017.875 â‚¬</t>
+          <t>15.017.875 €</t>
         </is>
       </c>
     </row>

</xml_diff>